<commit_message>
config changed, style added
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\UiPath\PWC-Arbitr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8424D3F0-B171-4C5B-891E-BF2C7CD72AEC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D0E7D1-0A74-430C-98BD-D240A5EB4DF2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16185" windowHeight="8325" xr2:uid="{88EBA8B9-481D-4AB2-8B1F-5CABE7CAB6CB}"/>
+    <workbookView xWindow="1808" yWindow="1808" windowWidth="17880" windowHeight="10417" activeTab="1" xr2:uid="{7D3A88F7-2D77-4A6B-AC43-53B4F77A4F2C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Лист1" sheetId="1" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+  <si>
+    <t>Статус</t>
+  </si>
   <si>
     <t>Название компании</t>
   </si>
@@ -49,12 +52,15 @@
     <t>Ссылка</t>
   </si>
   <si>
-    <t>Статус</t>
+    <t>Обнаружено судебное дело (см. ссылку)</t>
   </si>
   <si>
     <t>ООО  "СЕГМЕНТЭНЕРГО"</t>
   </si>
   <si>
+    <t>5048028638</t>
+  </si>
+  <si>
     <t>https://kad.arbitr.ru/Card/8d2b2994-f907-46b9-a543-f31da906dfd3</t>
   </si>
   <si>
@@ -67,6 +73,9 @@
     <t>ООО «Воздушные ворота Северной Столицы»</t>
   </si>
   <si>
+    <t>https://kad.arbitr.ru/Card/e822be21-090a-45ad-83d5-e16c28e2ab38</t>
+  </si>
+  <si>
     <t>https://kad.arbitr.ru/Card/ae2b2475-6cf3-4178-91d6-98831f34df13</t>
   </si>
   <si>
@@ -76,23 +85,20 @@
     <t>https://kad.arbitr.ru/Card/fe6cd8b9-29ff-4f22-9878-b65074ce60f2</t>
   </si>
   <si>
-    <t>Обнаружено судебное дело (см. ссылку)</t>
-  </si>
-  <si>
-    <t>https://kad.arbitr.ru/Card/e822be21-090a-45ad-83d5-e16c28e2ab38</t>
+    <t>Судебных дел не обнаружено</t>
   </si>
   <si>
     <t>ООО "Noname"</t>
-  </si>
-  <si>
-    <t>Судебных дел не обнаружено</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,12 +108,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -140,22 +152,73 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{A07DC705-8F83-436D-9DC0-7CEB9D95F573}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -166,6 +229,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E450E0FB-801A-4EF3-86B7-1B193147E176}" name="Таблица1" displayName="Таблица1" ref="A1:F8" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A1:F8" xr:uid="{A0B55D26-6055-4627-910F-968D42A44530}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{1ADF668D-B181-4150-BDF7-C27EE2BD4E56}" name="Статус" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FAEE9F02-7D94-436C-8783-84D942DF5807}" name="Название компании" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{BD3110E1-9235-4132-94D9-30DB70ACFE64}" name="ИНН" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A903184A-4DF7-402D-AF87-53E222BB10DA}" name="Начало периода" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{ADE466B0-E602-436E-A022-34ED2E2C0497}" name="Окончание периода" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{03A70303-5AF3-4319-8860-AD34F56F437F}" name="Ссылка" dataDxfId="0" dataCellStyle="Гиперссылка"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,244 +542,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C8FDB7-D81B-4763-A619-C6B6FAEF28F1}">
-  <dimension ref="A1:F23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="22.9296875" customWidth="1"/>
-    <col min="3" max="3" width="21.06640625" customWidth="1"/>
-    <col min="4" max="4" width="20.53125" customWidth="1"/>
-    <col min="5" max="5" width="24.796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>5048028638</v>
-      </c>
-      <c r="D2" s="1">
-        <v>36914</v>
-      </c>
-      <c r="E2" s="2">
-        <v>43458</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>7838412492</v>
-      </c>
-      <c r="D3" s="1">
-        <v>32885</v>
-      </c>
-      <c r="E3" s="1">
-        <v>43366</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1">
-        <v>7703590927</v>
-      </c>
-      <c r="D4" s="1">
-        <v>42858</v>
-      </c>
-      <c r="E4" s="1">
-        <v>43081</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1">
-        <v>7703590927</v>
-      </c>
-      <c r="D5" s="1">
-        <v>42858</v>
-      </c>
-      <c r="E5" s="1">
-        <v>43081</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>7703590927</v>
-      </c>
-      <c r="D6" s="1">
-        <v>42858</v>
-      </c>
-      <c r="E6" s="1">
-        <v>43081</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1">
-        <v>7703590927</v>
-      </c>
-      <c r="D7" s="1">
-        <v>42858</v>
-      </c>
-      <c r="E7" s="1">
-        <v>43081</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4352354308</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://kad.arbitr.ru/Card/8d2b2994-f907-46b9-a543-f31da906dfd3" xr:uid="{D9683C9E-538B-4973-BE93-08EB0679DC79}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7484E86C-8F1D-4632-9892-7E25360594B3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE7E14-0CBD-4FAD-9309-B970C0A1CF12}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -710,4 +551,183 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C6F979-C215-4513-B75D-F16218407316}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20.53125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.1328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.86328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.06640625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
+        <v>36914</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43458</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7838412492</v>
+      </c>
+      <c r="D3" s="6">
+        <v>32885</v>
+      </c>
+      <c r="E3" s="6">
+        <v>43366</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>7703590927</v>
+      </c>
+      <c r="D4" s="6">
+        <v>42858</v>
+      </c>
+      <c r="E4" s="6">
+        <v>43081</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7703590927</v>
+      </c>
+      <c r="D5" s="6">
+        <v>42858</v>
+      </c>
+      <c r="E5" s="6">
+        <v>43081</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7703590927</v>
+      </c>
+      <c r="D6" s="6">
+        <v>42858</v>
+      </c>
+      <c r="E6" s="6">
+        <v>43081</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7703590927</v>
+      </c>
+      <c r="D7" s="6">
+        <v>42858</v>
+      </c>
+      <c r="E7" s="6">
+        <v>43081</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4352354308</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
config updated, server error catched
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,31 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\UiPath\PWC-Arbitr\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D0E7D1-0A74-430C-98BD-D240A5EB4DF2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F484E7-74D2-4544-B5A6-799FE1114F3D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1808" yWindow="1808" windowWidth="17880" windowHeight="10417" activeTab="1" xr2:uid="{7D3A88F7-2D77-4A6B-AC43-53B4F77A4F2C}"/>
+    <workbookView xWindow="675" yWindow="2280" windowWidth="10710" windowHeight="10417" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Result" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -34,22 +22,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
+    <t>Название компании</t>
+  </si>
+  <si>
+    <t>ИНН</t>
+  </si>
+  <si>
+    <t>Начало периода</t>
+  </si>
+  <si>
+    <t>Окончание периода</t>
+  </si>
+  <si>
+    <t>Ссылка</t>
+  </si>
+  <si>
     <t>Статус</t>
-  </si>
-  <si>
-    <t>Название компании</t>
-  </si>
-  <si>
-    <t>ИНН</t>
-  </si>
-  <si>
-    <t>Начало периода</t>
-  </si>
-  <si>
-    <t>Окончание периода</t>
-  </si>
-  <si>
-    <t>Ссылка</t>
   </si>
   <si>
     <t>Обнаружено судебное дело (см. ссылку)</t>
@@ -95,18 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,40 +129,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1" xr:uid="{A07DC705-8F83-436D-9DC0-7CEB9D95F573}"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -232,24 +203,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E450E0FB-801A-4EF3-86B7-1B193147E176}" name="Таблица1" displayName="Таблица1" ref="A1:F8" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83986B22-3B61-405F-88BB-9684BD4B813A}" name="Таблица1" displayName="Таблица1" ref="A1:F8" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F8" xr:uid="{A0B55D26-6055-4627-910F-968D42A44530}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1ADF668D-B181-4150-BDF7-C27EE2BD4E56}" name="Статус" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{FAEE9F02-7D94-436C-8783-84D942DF5807}" name="Название компании" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{BD3110E1-9235-4132-94D9-30DB70ACFE64}" name="ИНН" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{A903184A-4DF7-402D-AF87-53E222BB10DA}" name="Начало периода" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{ADE466B0-E602-436E-A022-34ED2E2C0497}" name="Окончание периода" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{03A70303-5AF3-4319-8860-AD34F56F437F}" name="Ссылка" dataDxfId="0" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="1" xr3:uid="{CFB6E728-64A8-4ADF-BDB3-A1E196E36295}" name="Статус" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8AB05E53-751C-4C31-98E0-0B3AB86B97AF}" name="Название компании" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{2D836B73-6073-464E-8A65-45719478164D}" name="ИНН" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{70556501-B593-419F-9AAA-564826304ACB}" name="Начало периода" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{B63A20C1-7098-4D7C-AA83-8249B66CCA46}" name="Окончание периода" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{4338B633-B471-472B-986F-66F32040775F}" name="Ссылка" dataDxfId="0" dataCellStyle="Гиперссылка"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -263,7 +234,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -275,7 +246,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -287,12 +258,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -322,29 +293,12 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -374,26 +328,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -542,56 +479,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE7E14-0CBD-4FAD-9309-B970C0A1CF12}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C6F979-C215-4513-B75D-F16218407316}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702B5DF7-8DAE-4FF5-87DD-7EBCF11EC697}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.53125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.1328125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.265625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.86328125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="5"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="16.1328125" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
+    <col min="4" max="4" width="16.1328125" customWidth="1"/>
+    <col min="5" max="5" width="18.1328125" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="93.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -611,7 +537,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -620,10 +546,10 @@
       <c r="C3" s="2">
         <v>7838412492</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>32885</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
         <v>43366</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -631,7 +557,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -640,10 +566,10 @@
       <c r="C4" s="2">
         <v>7703590927</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>42858</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
         <v>43081</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -651,7 +577,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -660,10 +586,10 @@
       <c r="C5" s="2">
         <v>7703590927</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>42858</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <v>43081</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -671,7 +597,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -680,10 +606,10 @@
       <c r="C6" s="2">
         <v>7703590927</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>42858</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="3">
         <v>43081</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -691,7 +617,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.45">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -700,10 +626,10 @@
       <c r="C7" s="2">
         <v>7703590927</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>42858</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
         <v>43081</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -711,7 +637,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -720,8 +646,8 @@
       <c r="C8" s="2">
         <v>4352354308</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
error handling (update #1)
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FDBF0A-4CB8-4594-918C-6D948A74609B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4858BF8C-B8C3-4205-9A3B-120D75B4881F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="675" yWindow="2280" windowWidth="10710" windowHeight="10417" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="70">
   <si>
     <t>Название компании</t>
   </si>
@@ -55,10 +55,181 @@
     <t>ООО "ЕВРОТРАНС"</t>
   </si>
   <si>
+    <t>https://kad.arbitr.ru/Card/780836a7-5023-4339-8046-faa7f0da936e</t>
+  </si>
+  <si>
     <t>ООО «Воздушные ворота Северной Столицы»</t>
   </si>
   <si>
+    <t>https://kad.arbitr.ru/Card/e822be21-090a-45ad-83d5-e16c28e2ab38</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/ae2b2475-6cf3-4178-91d6-98831f34df13</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/3a932120-5fd6-47c4-9449-c3fb6a45f257</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/fe6cd8b9-29ff-4f22-9878-b65074ce60f2</t>
+  </si>
+  <si>
+    <t>Судебных дел не обнаружено</t>
+  </si>
+  <si>
     <t>ООО "Noname"</t>
+  </si>
+  <si>
+    <t>ПАО "Газпром"</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/69b2d3bb-bfe3-4188-ae8b-31fc618fa71e</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/dd80dea5-0346-4d04-babe-a90c8ae881ae</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/65700c1e-9bb4-496f-bc5c-d1489cd04234</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/dbaf67a6-6284-4b4a-9fc1-684a10ff171d</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/6bf3545a-5bf7-43c6-ab18-df0c294e41fc</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/05df5e0d-63b2-4338-bf60-81c6af8210ce</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/f33e9663-5bf7-4add-bf56-6b963610e328</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/f9d9f6ea-8ccb-45e4-9866-a72b854106ce</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/e6f60b4e-e2e6-495a-b604-6bd49b49c5ea</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/15c84220-8465-4245-a278-bf0dce7daadc</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/c139b0e9-cbdb-474a-93f0-c9ea731e9a4c</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/6be51bc4-bc09-46af-b35c-f4ce9e72196d</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/e011bf1b-6893-4625-9dfb-51d5d0380f59</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/fbe6f3fe-2c96-44cf-bf85-0dde665bb955</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/d602b39f-8e4d-4796-9d95-4066a01dc85d</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/f6e714ac-5714-4b1f-bd01-2f906f32f778</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/6bb158cb-b099-49e0-aae6-e49cde2cb50f</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/963a9172-3230-45a9-88c1-8d10dcb8eaa4</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/1494fbb2-e183-4238-8dd9-97a0a9b8865b</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/68710027-6409-4249-a763-7c1696d9abc6</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/1e327842-e6fe-493b-ab67-f6491cf757fe</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/7ffab5db-e423-456b-897b-a0acef229579</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/ad4d45cc-5c7e-48e2-aa6a-3fcfde3eafae</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/89e6fda0-2a41-4108-ba80-db16ce8c9ff5</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/4937f5fa-6c67-40f2-ac58-9eeb00779a7b</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/454a759f-c22e-4520-92ab-1f068f8a3ca7</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/00fdcf34-bdcb-4149-b59d-5af75169311a</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/c6bad8b6-ae08-4b47-8592-2ea1fabc9b04</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/9ac156fc-a232-42ed-aafd-f45fdca05111</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/ed2ebfe1-87e5-4fa0-93af-8644dd66c5fa</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/e5654180-cc87-4c83-b2ba-f48402cf952e</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/98c8622f-c798-491c-86b3-1ea6634e4813</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/05a22775-21fe-49fe-a070-3fa0e170aa40</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/54090a36-b368-4344-98d0-00ad85aa8d89</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/519adfe6-51b5-4b14-8aef-edcbd86286e9</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/a6637c3a-85a0-4296-84d2-9df21f774722</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/bddcf9e5-9719-4f8a-b2bf-132fef7fe173</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/741e3ad2-1cb2-4d20-903c-62d827156a0c</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/b599a744-e343-420f-883f-c08293ff829c</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/fe4d6608-8c46-4af3-b9fe-f4b7286c8f60</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/3f121bc1-d516-49ae-9e5e-05527528559c</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/93efd27b-e9bc-4b0f-b3f7-deac7ec6af21</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/74a22f65-16ba-417b-b3e6-48676043eafe</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/7d5612a4-fa80-4a60-9350-f260b705f4eb</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/d09bbca7-e3a9-483a-a9b8-eea5477d548a</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/4f0a1a93-3c42-4af6-abaf-02de4ee44426</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/bb2e38e3-fa5f-4819-86c1-caa37df731e6</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/1c5e36cf-757b-42d1-bfc3-854572b1db43</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/bdb58721-1438-496c-bc7c-0a22cd810700</t>
+  </si>
+  <si>
+    <t>https://kad.arbitr.ru/Card/0785612c-1490-409d-bc3d-ef9c749a8386</t>
   </si>
 </sst>
 </file>
@@ -82,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +263,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -124,6 +301,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -176,8 +356,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83986B22-3B61-405F-88BB-9684BD4B813A}" name="Таблица1" displayName="Таблица1" ref="A1:F5" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="A1:F5" xr:uid="{A0B55D26-6055-4627-910F-968D42A44530}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{83986B22-3B61-405F-88BB-9684BD4B813A}" name="Таблица1" displayName="Таблица1" ref="A1:F58" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A1:F58" xr:uid="{A0B55D26-6055-4627-910F-968D42A44530}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CFB6E728-64A8-4ADF-BDB3-A1E196E36295}" name="Статус" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{8AB05E53-751C-4C31-98E0-0B3AB86B97AF}" name="Название компании" dataDxfId="4"/>
@@ -453,7 +633,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702B5DF7-8DAE-4FF5-87DD-7EBCF11EC697}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
@@ -526,7 +706,7 @@
         <v>43366</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.45">
@@ -534,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>7703590927</v>
@@ -546,7 +726,7 @@
         <v>43081</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.45">
@@ -557,12 +737,1070 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
+        <v>7703590927</v>
+      </c>
+      <c r="D5" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7703590927</v>
+      </c>
+      <c r="D6" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E6" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7703590927</v>
+      </c>
+      <c r="D7" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E7" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2">
         <v>4352354308</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D9" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E9" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D10" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E10" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D11" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E11" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D12" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E12" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D13" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E13" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D14" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E14" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D15" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E15" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D16" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E16" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D17" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E17" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D18" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E18" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D19" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E19" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D20" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E20" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D21" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E21" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D22" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E22" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D23" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E23" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D24" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E24" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D25" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E25" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D26" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E26" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D27" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E27" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D28" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E28" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D29" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E29" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D30" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E30" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D31" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E31" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D32" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E32" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D33" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E33" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D34" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E34" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D35" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E35" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D36" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E36" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D37" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E37" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D38" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E38" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D39" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E39" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D40" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E40" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D41" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E41" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D42" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E42" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D43" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E43" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D44" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E44" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D45" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E45" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D46" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E46" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D47" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E47" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D48" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E48" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D49" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E49" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D50" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E50" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D51" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E51" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D52" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E52" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A53" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D53" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E53" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D54" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E54" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A55" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D55" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E55" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A56" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D56" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E56" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A57" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D57" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E57" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+      <c r="A58" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="2">
+        <v>7736050003</v>
+      </c>
+      <c r="D58" s="3">
+        <v>42858</v>
+      </c>
+      <c r="E58" s="3">
+        <v>43081</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>